<commit_message>
Faturação a acontecer!! Vários contadores na mesma fatura causa problemas!!
</commit_message>
<xml_diff>
--- a/ASSREG-Faturacao/Mapa de contadores.xlsx
+++ b/ASSREG-Faturacao/Mapa de contadores.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39494F9-B318-4934-8F0C-26BF21083CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6E4EC3-624B-4BBE-8820-5B9F8A1186F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -415,56 +415,56 @@
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -818,7 +818,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T11" sqref="T11"/>
+      <selection pane="bottomLeft" activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -839,26 +839,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="50"/>
-      <c r="R1" s="50"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
     </row>
     <row r="2" spans="1:29" ht="21" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="3" t="s">
@@ -883,26 +883,26 @@
       <c r="R2" s="26"/>
     </row>
     <row r="3" spans="1:29" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="51"/>
-      <c r="P3" s="51"/>
-      <c r="Q3" s="51"/>
-      <c r="R3" s="51"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
     </row>
     <row r="4" spans="1:29" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E4" s="25" t="s">
@@ -975,13 +975,13 @@
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A6" s="35">
+      <c r="A6" s="37">
         <v>1</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="37" t="s">
         <v>51</v>
       </c>
       <c r="D6" s="6" t="s">
@@ -990,98 +990,98 @@
       <c r="E6" s="14">
         <v>4.1399999999999999E-2</v>
       </c>
-      <c r="F6" s="35" t="s">
+      <c r="F6" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="G6" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="J6" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="K6" s="45">
+      <c r="G6" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" s="48">
         <v>13139080205</v>
       </c>
-      <c r="L6" s="45">
+      <c r="L6" s="48">
         <v>1143</v>
       </c>
-      <c r="M6" s="43" t="s">
+      <c r="M6" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="N6" s="40">
+      <c r="N6" s="42">
         <v>1042</v>
       </c>
-      <c r="O6" s="38">
+      <c r="O6" s="40">
         <v>44617</v>
       </c>
-      <c r="P6" s="40">
+      <c r="P6" s="42">
         <v>1046</v>
       </c>
-      <c r="Q6" s="38">
+      <c r="Q6" s="40">
         <v>44890</v>
       </c>
-      <c r="R6" s="40">
+      <c r="R6" s="42">
         <v>1459</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A7" s="36"/>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
+      <c r="A7" s="35"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
       <c r="D7" s="6" t="s">
         <v>24</v>
       </c>
       <c r="E7" s="14">
         <v>2.8199999999999999E-2</v>
       </c>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36"/>
-      <c r="K7" s="46"/>
-      <c r="L7" s="46"/>
-      <c r="M7" s="49"/>
-      <c r="N7" s="42"/>
-      <c r="O7" s="48"/>
-      <c r="P7" s="42"/>
-      <c r="Q7" s="48"/>
-      <c r="R7" s="42"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="49"/>
+      <c r="L7" s="49"/>
+      <c r="M7" s="47"/>
+      <c r="N7" s="43"/>
+      <c r="O7" s="41"/>
+      <c r="P7" s="43"/>
+      <c r="Q7" s="41"/>
+      <c r="R7" s="43"/>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A8" s="36"/>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
       <c r="D8" s="6" t="s">
         <v>21</v>
       </c>
       <c r="E8" s="14">
         <v>3.3399999999999999E-2</v>
       </c>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="47"/>
-      <c r="L8" s="47"/>
-      <c r="M8" s="44"/>
-      <c r="N8" s="41"/>
-      <c r="O8" s="39"/>
-      <c r="P8" s="41"/>
-      <c r="Q8" s="39"/>
-      <c r="R8" s="41"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="51"/>
+      <c r="N8" s="45"/>
+      <c r="O8" s="44"/>
+      <c r="P8" s="45"/>
+      <c r="Q8" s="44"/>
+      <c r="R8" s="45"/>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A9" s="36"/>
-      <c r="B9" s="36"/>
-      <c r="C9" s="37"/>
+      <c r="A9" s="35"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="36"/>
       <c r="D9" s="6" t="s">
         <v>10</v>
       </c>
@@ -1129,9 +1129,9 @@
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A10" s="36"/>
-      <c r="B10" s="36"/>
-      <c r="C10" s="36" t="s">
+      <c r="A10" s="35"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35" t="s">
         <v>51</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -1140,97 +1140,97 @@
       <c r="E10" s="14">
         <v>2.4400000000000002E-2</v>
       </c>
-      <c r="F10" s="35" t="s">
+      <c r="F10" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="G10" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="H10" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="I10" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="J10" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="K10" s="45">
+      <c r="G10" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="K10" s="48">
         <v>13139080143</v>
       </c>
-      <c r="L10" s="45">
+      <c r="L10" s="48">
         <v>1037</v>
       </c>
-      <c r="M10" s="43" t="s">
+      <c r="M10" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="N10" s="40">
+      <c r="N10" s="42">
         <v>1529</v>
       </c>
-      <c r="O10" s="38">
+      <c r="O10" s="40">
         <v>44617</v>
       </c>
-      <c r="P10" s="40">
+      <c r="P10" s="42">
         <v>1529</v>
       </c>
-      <c r="Q10" s="38">
+      <c r="Q10" s="40">
         <v>44890</v>
       </c>
-      <c r="R10" s="40">
+      <c r="R10" s="42">
         <v>1826</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A11" s="36"/>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
+      <c r="A11" s="35"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
       <c r="D11" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="14">
         <v>2.8199999999999999E-2</v>
       </c>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="36"/>
-      <c r="K11" s="46"/>
-      <c r="L11" s="46"/>
-      <c r="M11" s="49"/>
-      <c r="N11" s="42"/>
-      <c r="O11" s="48"/>
-      <c r="P11" s="42"/>
-      <c r="Q11" s="48"/>
-      <c r="R11" s="42"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="49"/>
+      <c r="L11" s="49"/>
+      <c r="M11" s="47"/>
+      <c r="N11" s="43"/>
+      <c r="O11" s="41"/>
+      <c r="P11" s="43"/>
+      <c r="Q11" s="41"/>
+      <c r="R11" s="43"/>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A12" s="36"/>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
+      <c r="A12" s="35"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
       <c r="D12" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E12" s="14">
         <v>1.18E-2</v>
       </c>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="36"/>
-      <c r="K12" s="46"/>
-      <c r="L12" s="46"/>
-      <c r="M12" s="49"/>
-      <c r="N12" s="42"/>
-      <c r="O12" s="48"/>
-      <c r="P12" s="42"/>
-      <c r="Q12" s="48"/>
-      <c r="R12" s="42"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="49"/>
+      <c r="L12" s="49"/>
+      <c r="M12" s="47"/>
+      <c r="N12" s="43"/>
+      <c r="O12" s="41"/>
+      <c r="P12" s="43"/>
+      <c r="Q12" s="41"/>
+      <c r="R12" s="43"/>
     </row>
     <row r="13" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="36"/>
-      <c r="B13" s="36"/>
+      <c r="A13" s="35"/>
+      <c r="B13" s="35"/>
       <c r="C13" s="8"/>
       <c r="D13" s="6" t="s">
         <v>8</v>
@@ -1290,9 +1290,9 @@
       <c r="AC13"/>
     </row>
     <row r="14" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="36"/>
-      <c r="B14" s="36"/>
-      <c r="C14" s="35" t="s">
+      <c r="A14" s="35"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="37" t="s">
         <v>45</v>
       </c>
       <c r="D14" s="6" t="s">
@@ -1353,9 +1353,9 @@
       <c r="AC14"/>
     </row>
     <row r="15" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="37"/>
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
+      <c r="A15" s="36"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
       <c r="D15" s="6" t="s">
         <v>14</v>
       </c>
@@ -1414,13 +1414,13 @@
       <c r="AC15"/>
     </row>
     <row r="16" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="35">
+      <c r="A16" s="37">
         <v>1</v>
       </c>
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="35" t="s">
+      <c r="C16" s="37" t="s">
         <v>44</v>
       </c>
       <c r="D16" s="6" t="s">
@@ -1481,9 +1481,9 @@
       <c r="AC16"/>
     </row>
     <row r="17" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="37"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
+      <c r="A17" s="36"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
       <c r="D17" s="6" t="s">
         <v>25</v>
       </c>
@@ -1542,13 +1542,13 @@
       <c r="AC17"/>
     </row>
     <row r="18" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="35">
+      <c r="A18" s="37">
         <v>1</v>
       </c>
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="35" t="s">
+      <c r="C18" s="37" t="s">
         <v>44</v>
       </c>
       <c r="D18" s="6" t="s">
@@ -1609,9 +1609,9 @@
       <c r="AC18"/>
     </row>
     <row r="19" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
-      <c r="C19" s="37"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="36"/>
       <c r="D19" s="6" t="s">
         <v>29</v>
       </c>
@@ -1670,9 +1670,9 @@
       <c r="AC19"/>
     </row>
     <row r="20" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="36"/>
-      <c r="B20" s="36"/>
-      <c r="C20" s="35" t="s">
+      <c r="A20" s="35"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="37" t="s">
         <v>45</v>
       </c>
       <c r="D20" s="6" t="s">
@@ -1733,9 +1733,9 @@
       <c r="AC20"/>
     </row>
     <row r="21" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="36"/>
-      <c r="B21" s="36"/>
-      <c r="C21" s="36"/>
+      <c r="A21" s="35"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="35"/>
       <c r="D21" s="6" t="s">
         <v>33</v>
       </c>
@@ -1794,9 +1794,9 @@
       <c r="AC21"/>
     </row>
     <row r="22" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="37"/>
-      <c r="B22" s="37"/>
-      <c r="C22" s="37"/>
+      <c r="A22" s="36"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="36"/>
       <c r="D22" s="6" t="s">
         <v>35</v>
       </c>
@@ -1828,19 +1828,19 @@
         <v>36</v>
       </c>
       <c r="N22" s="29">
-        <v>2411</v>
+        <v>2500</v>
       </c>
       <c r="O22" s="2">
         <v>44613</v>
       </c>
       <c r="P22" s="31">
-        <v>2488</v>
+        <v>7800</v>
       </c>
       <c r="Q22" s="2">
         <v>44888</v>
       </c>
       <c r="R22" s="31">
-        <v>3409</v>
+        <v>12000</v>
       </c>
       <c r="S22"/>
       <c r="T22"/>
@@ -1870,11 +1870,19 @@
     <mergeCell ref="J6:J8"/>
     <mergeCell ref="F10:F12"/>
     <mergeCell ref="G10:G12"/>
+    <mergeCell ref="N10:N12"/>
+    <mergeCell ref="O10:O12"/>
+    <mergeCell ref="P10:P12"/>
+    <mergeCell ref="N6:N8"/>
     <mergeCell ref="K6:K8"/>
     <mergeCell ref="L6:L8"/>
     <mergeCell ref="M6:M8"/>
     <mergeCell ref="K10:K12"/>
     <mergeCell ref="L10:L12"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="C18:C19"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="A3:R3"/>
     <mergeCell ref="C10:C12"/>
@@ -1887,20 +1895,12 @@
     <mergeCell ref="Q6:Q8"/>
     <mergeCell ref="R6:R8"/>
     <mergeCell ref="M10:M12"/>
-    <mergeCell ref="N10:N12"/>
-    <mergeCell ref="O10:O12"/>
-    <mergeCell ref="P10:P12"/>
-    <mergeCell ref="N6:N8"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="C14:C15"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="C16:C17"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="B18:B22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="C14:C15"/>
   </mergeCells>
   <pageMargins left="0.31496062992125984" right="0.11811023622047245" top="0.74803149606299213" bottom="0.94488188976377963" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="8" scale="99" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>